<commit_message>
Update Taiwan.xlsx from scraper run
</commit_message>
<xml_diff>
--- a/Taiwan.xlsx
+++ b/Taiwan.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,1857 +434,1488 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Month</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2015 JAN</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2015 JAN</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>66,452</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2015 FEB</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2015 FEB</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>66,762</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2015 MAR</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2015 MAR</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>66,699</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2015 APR</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2015 APR</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>65,680</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2015 MAY</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2015 MAY</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>66,121</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2015 JUN</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2015 JUN</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
           <t>66,070</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2015 JUL</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2015 JUL</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
           <t>65,870</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2015 AUG</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2015 AUG</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>65,825</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2015 SEP</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2015 SEP</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
           <t>65,734</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2015 OCT</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2015 OCT</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
           <t>65,683</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2015 NOV</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2015 NOV</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>65,678</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2015 DEC</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2015 DEC</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
           <t>65,927</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2016 JAN</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2016 JAN</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
           <t>66,410</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2016 FEB</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2016 FEB</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>66,391</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2016 MAR</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2016 MAR</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
           <t>66,356</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2016 APR</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2016 APR</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
           <t>66,257</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2016 MAY</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2016 MAY</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
           <t>65,320</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2016 JUN</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2016 JUN</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
           <t>64,891</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2016 JUL</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2016 JUL</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
           <t>64,872</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2016 AUG</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2016 AUG</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
           <t>64,006</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2016 SEP</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2016 SEP</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
           <t>64,354</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2016 OCT</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2016 OCT</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
           <t>64,178</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2016 NOV</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2016 NOV</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
           <t>64,065</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2016 DEC</t>
+        </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2016 DEC</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
           <t>64,301</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2017 JAN</t>
+        </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2017 JAN</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
           <t>64,756</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2017 FEB</t>
+        </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2017 FEB</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
           <t>64,632</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2017 MAR</t>
+        </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2017 MAR</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
           <t>64,062</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2017 APR</t>
+        </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2017 APR</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
           <t>64,534</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2017 MAY</t>
+        </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2017 MAY</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
           <t>63,349</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2017 JUN</t>
+        </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2017 JUN</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
           <t>64,324</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2017 JUL</t>
+        </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2017 JUL</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
           <t>64,270</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2017 AUG</t>
+        </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2017 AUG</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
           <t>64,167</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2017 SEP</t>
+        </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2017 SEP</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
           <t>63,961</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2017 OCT</t>
+        </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2017 OCT</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
           <t>63,956</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2017 NOV</t>
+        </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2017 NOV</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
           <t>63,821</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2017 DEC</t>
+        </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2017 DEC</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
           <t>64,042</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2018 JAN</t>
+        </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2018 JAN</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
           <t>64,350</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2018 FEB</t>
+        </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2018 FEB</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
           <t>64,700</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2018 MAR</t>
+        </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2018 MAR</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
           <t>64,245</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2018 APR</t>
+        </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2018 APR</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
           <t>64,523</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2018 MAY</t>
+        </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2018 MAY</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
           <t>62,873</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2018 JUN</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2018 JUN</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
           <t>64,385</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2018 JUL</t>
+        </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2018 JUL</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
           <t>64,259</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2018 AUG</t>
+        </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2018 AUG</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
           <t>65,696</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2018 SEP</t>
+        </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2018 SEP</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
           <t>65,642</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2018 OCT</t>
+        </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2018 OCT</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
           <t>65,675</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2018 NOV</t>
+        </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2018 NOV</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
           <t>65,627</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2018 DEC</t>
+        </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2018 DEC</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
           <t>65,431</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2019 JAN</t>
+        </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2019 JAN</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
           <t>66,361</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2019 FEB</t>
+        </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2019 FEB</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
           <t>65,956</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2019 MAR</t>
+        </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2019 MAR</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
           <t>66,024</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2019 APR</t>
+        </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2019 APR</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
           <t>64,636</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2019 MAY</t>
+        </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2019 MAY</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
           <t>65,449</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2019 JUN</t>
+        </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2019 JUN</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
           <t>65,372</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2019 JUL</t>
+        </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2019 JUL</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
           <t>65,300</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2019 AUG</t>
+        </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2019 AUG</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
           <t>65,365</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2019 SEP</t>
+        </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2019 SEP</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
           <t>64,946</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2019 OCT</t>
+        </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2019 OCT</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
           <t>65,040</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2019 NOV</t>
+        </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2019 NOV</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
           <t>64,933</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2019 DEC</t>
+        </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2019 DEC</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
           <t>64,270</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2020 JAN</t>
+        </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2020 JAN</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
           <t>65,039</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2020 FEB</t>
+        </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2020 FEB</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
           <t>65,216</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2020 MAR</t>
+        </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2020 MAR</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
           <t>65,049</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2020 APR</t>
+        </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2020 APR</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
           <t>64,724</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2020 MAY</t>
+        </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2020 MAY</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
           <t>64,650</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>65</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2020 JUN</t>
+        </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2020 JUN</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
           <t>65,048</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2020 JUL</t>
+        </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2020 JUL</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
           <t>64,697</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2020 AUG</t>
+        </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2020 AUG</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
           <t>65,197</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2020 SEP</t>
+        </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2020 SEP</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
           <t>65,060</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2020 OCT</t>
+        </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2020 OCT</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
           <t>65,081</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2020 NOV</t>
+        </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2020 NOV</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
           <t>64,829</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2020 DEC</t>
+        </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2020 DEC</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
           <t>64,851</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2021 JAN</t>
+        </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2021 JAN</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
           <t>65,373</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2021 FEB</t>
+        </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2021 FEB</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
           <t>65,451</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2021 MAR</t>
+        </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2021 MAR</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
           <t>65,478</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2021 APR</t>
+        </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2021 APR</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
           <t>65,522</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2021 MAY</t>
+        </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2021 MAY</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
           <t>64,002</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2021 JUN</t>
+        </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2021 JUN</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
           <t>64,738</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2021 JUL</t>
+        </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2021 JUL</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
           <t>64,140</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>79</v>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2021 AUG</t>
+        </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2021 AUG</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
           <t>64,267</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>80</v>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2021 SEP</t>
+        </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2021 SEP</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
           <t>64,162</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>81</v>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2021 OCT</t>
+        </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2021 OCT</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
           <t>64,135</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>82</v>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2021 NOV</t>
+        </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2021 NOV</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
           <t>64,134</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>83</v>
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2021 DEC</t>
+        </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2021 DEC</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
           <t>63,600</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>84</v>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2022 JAN</t>
+        </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2022 JAN</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
           <t>65,029</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>85</v>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2022 FEB</t>
+        </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2022 FEB</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
           <t>64,801</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>86</v>
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2022 MAR</t>
+        </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2022 MAR</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
           <t>64,860</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>87</v>
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2022 APR</t>
+        </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2022 APR</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
           <t>64,954</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>88</v>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2022 MAY</t>
+        </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2022 MAY</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
           <t>64,171</t>
         </is>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>89</v>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2022 JUN</t>
+        </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2022 JUN</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
           <t>63,974</t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>90</v>
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2022 JUL</t>
+        </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2022 JUL</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
           <t>65,372</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2022 AUG</t>
+        </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2022 AUG</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
           <t>65,368</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2022 SEP</t>
+        </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2022 SEP</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
           <t>65,240</t>
         </is>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2022 OCT</t>
+        </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2022 OCT</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
           <t>65,502</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2022 NOV</t>
+        </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2022 NOV</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
           <t>65,227</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>95</v>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2022 DEC</t>
+        </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2022 DEC</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
           <t>65,905</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>96</v>
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2023 JAN</t>
+        </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2023 JAN</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
           <t>66,281</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2023 FEB</t>
+        </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2023 FEB</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
           <t>66,270</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2023 MAR</t>
+        </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2023 MAR</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
           <t>66,215</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2023 APR</t>
+        </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2023 APR</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
           <t>66,405</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2023 MAY</t>
+        </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2023 MAY</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
           <t>65,972</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2023 JUN</t>
+        </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2023 JUN</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
           <t>65,849</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2023 JUL</t>
+        </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2023 JUL</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
           <t>65,581</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2023 AUG</t>
+        </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2023 AUG</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
           <t>65,749</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2023 SEP</t>
+        </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2023 SEP</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
           <t>65,521</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2023 OCT</t>
+        </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2023 OCT</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
           <t>65,700</t>
         </is>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2023 NOV</t>
+        </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2023 NOV</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
           <t>65,558</t>
         </is>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2023 DEC</t>
+        </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2023 DEC</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
           <t>65,697</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>108</v>
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024 JAN</t>
+        </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2024 JAN</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
           <t>66,716</t>
         </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024 FEB</t>
+        </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2024 FEB</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
           <t>66,756</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>110</v>
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024 MAR</t>
+        </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2024 MAR</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
           <t>66,222</t>
         </is>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>111</v>
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024 APR</t>
+        </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2024 APR</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
           <t>66,976</t>
         </is>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>112</v>
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024 MAY</t>
+        </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2024 MAY</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
           <t>65,484</t>
         </is>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024 JUN</t>
+        </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2024 JUN</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
           <t>66,909</t>
         </is>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024 JUL</t>
+        </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2024 JUL</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
           <t>65,959</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>115</v>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2024 AUG</t>
+        </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2024 AUG</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
           <t>65,435</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>116</v>
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2024 SEP</t>
+        </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2024 SEP</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
           <t>65,467</t>
         </is>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>117</v>
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024 OCT</t>
+        </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2024 OCT</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
           <t>65,129</t>
         </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>118</v>
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024 NOV</t>
+        </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2024 NOV</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
           <t>65,454</t>
         </is>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>119</v>
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2024 DEC</t>
+        </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2024 DEC</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
           <t>65,786</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>120</v>
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025 JAN</t>
+        </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>2025 JAN</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
           <t>66,424</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>121</v>
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025 FEB</t>
+        </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>2025 FEB</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
           <t>66,352</t>
         </is>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>122</v>
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025 MAR</t>
+        </is>
       </c>
       <c r="B124" t="inlineStr">
-        <is>
-          <t>2025 MAR</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
         <is>
           <t>66,420</t>
         </is>

</xml_diff>